<commit_message>
spelling error. Change Max Weights to 100% from 99.9999%.
</commit_message>
<xml_diff>
--- a/data/0_basic_asset_classes_constrained.xlsx
+++ b/data/0_basic_asset_classes_constrained.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6113f60f932799a7/1Evan/.efficient_frontier/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3A9D9B2-AFFA-450C-A7C8-172D2D497019}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A86655F-2FBF-4809-A238-99D83A1E3153}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Investments" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
-    <numFmt numFmtId="165" formatCode="#,##0.000%"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -132,11 +132,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,7 +446,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -467,7 +467,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -478,8 +478,8 @@
       <c r="B2" s="2">
         <v>0</v>
       </c>
-      <c r="C2" s="5">
-        <v>0.99999000000000005</v>
+      <c r="C2" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -489,7 +489,7 @@
       <c r="B3" s="2">
         <v>0</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="6">
         <v>0.75</v>
       </c>
     </row>
@@ -500,7 +500,7 @@
       <c r="B4" s="2">
         <v>0</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="6">
         <v>0.75</v>
       </c>
     </row>
@@ -511,7 +511,7 @@
       <c r="B5" s="2">
         <v>0</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="6">
         <v>0.25</v>
       </c>
     </row>
@@ -522,7 +522,7 @@
       <c r="B6" s="2">
         <v>0</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="6">
         <v>0.3</v>
       </c>
     </row>
@@ -533,7 +533,7 @@
       <c r="B7" s="2">
         <v>0</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="6">
         <v>0.15</v>
       </c>
     </row>
@@ -544,7 +544,7 @@
       <c r="B8" s="2">
         <v>0</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="6">
         <v>0.05</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed constraint on GLD in basic_asset_classes_constrained to 1%
</commit_message>
<xml_diff>
--- a/data/0_basic_asset_classes_constrained.xlsx
+++ b/data/0_basic_asset_classes_constrained.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6113f60f932799a7/1Evan/.efficient_frontier/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A86655F-2FBF-4809-A238-99D83A1E3153}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCD51309-6153-4071-B689-37222D779DC2}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00%"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -135,7 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -446,7 +446,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -545,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
force rebuild by streamlit.io
</commit_message>
<xml_diff>
--- a/data/0_basic_asset_classes_constrained.xlsx
+++ b/data/0_basic_asset_classes_constrained.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6113f60f932799a7/1Evan/.efficient_frontier/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCD51309-6153-4071-B689-37222D779DC2}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0CC1912-37E8-4EC5-896D-3F17D755FB09}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Investments" sheetId="1" r:id="rId1"/>
@@ -446,7 +446,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>